<commit_message>
Time to the sheet :beers:
</commit_message>
<xml_diff>
--- a/docs/Timesheets/Timesheet-Maximilian-Suitner.xlsx
+++ b/docs/Timesheets/Timesheet-Maximilian-Suitner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Projects\prodiga\docs\Timesheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84504CF7-E28A-43BF-ACB2-75682562437A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCC09BD-9997-47DE-A4CC-A1C0071090B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
   <si>
     <t>Datum</t>
   </si>
@@ -197,13 +197,46 @@
   <si>
     <t>5.4.2020</t>
   </si>
+  <si>
+    <t>13.4.2020</t>
+  </si>
+  <si>
+    <t>14.4.2020</t>
+  </si>
+  <si>
+    <t>Teambesprechung</t>
+  </si>
+  <si>
+    <t>15.4.2020</t>
+  </si>
+  <si>
+    <t>ErrorTrap fixen</t>
+  </si>
+  <si>
+    <t>16.4.2020</t>
+  </si>
+  <si>
+    <t>Booking vom Würfel schreiben</t>
+  </si>
+  <si>
+    <t>17.4.2020</t>
+  </si>
+  <si>
+    <t>DiceService more secure</t>
+  </si>
+  <si>
+    <t>18.4.2020</t>
+  </si>
+  <si>
+    <t>19.4.2020</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd\.mm\.yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy;@"/>
   </numFmts>
   <fonts count="10">
     <font>
@@ -318,10 +351,10 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -649,7 +682,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -889,7 +922,7 @@
         <v>40</v>
       </c>
       <c r="B17" s="6">
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
@@ -945,7 +978,7 @@
         <v>41</v>
       </c>
       <c r="B21" s="6">
-        <v>4.1666666666666664E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
@@ -983,32 +1016,102 @@
       </c>
     </row>
     <row r="24" spans="1:4">
-      <c r="B24" s="6"/>
-      <c r="D24" s="2"/>
+      <c r="A24" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="6">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="25" spans="1:4">
-      <c r="B25" s="6"/>
-      <c r="D25" s="2"/>
+      <c r="A25" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="6">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="26" spans="1:4">
-      <c r="B26" s="6"/>
-      <c r="D26" s="2"/>
+      <c r="A26" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="6">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="27" spans="1:4">
-      <c r="B27" s="6"/>
-      <c r="D27" s="2"/>
+      <c r="A27" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="6">
+        <v>0.125</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="28" spans="1:4">
-      <c r="B28" s="6"/>
-      <c r="D28" s="2"/>
+      <c r="A28" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="6">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="29" spans="1:4">
-      <c r="B29" s="6"/>
-      <c r="D29" s="2"/>
+      <c r="A29" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="6">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="30" spans="1:4">
-      <c r="B30" s="6"/>
-      <c r="D30" s="2"/>
+      <c r="A30" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" s="6">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="31" spans="1:4">
       <c r="B31" s="6"/>
@@ -4928,7 +5031,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E4555F9B-702D-FD4F-A0B2-5CBE96A3F479}">
           <x14:formula1>
             <xm:f>Tätigkeiten!$B$2:$B$12</xm:f>

</xml_diff>

<commit_message>
Time to the sheet
</commit_message>
<xml_diff>
--- a/docs/Timesheets/Timesheet-Maximilian-Suitner.xlsx
+++ b/docs/Timesheets/Timesheet-Maximilian-Suitner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Projects\prodiga\docs\Timesheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4494CD48-9437-44B8-9363-ADBF58948932}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F508748D-7E72-459A-958B-AE2AEA1A6AFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="69">
   <si>
     <t>Datum</t>
   </si>
@@ -235,6 +235,21 @@
   </si>
   <si>
     <t>LV Einheit</t>
+  </si>
+  <si>
+    <t>27.4.2020</t>
+  </si>
+  <si>
+    <t>23.4.2020</t>
+  </si>
+  <si>
+    <t>22.4.2020</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>24.4.2020</t>
   </si>
 </sst>
 </file>
@@ -688,7 +703,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
+      <selection pane="bottomRight" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
@@ -1147,67 +1162,107 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="2:4">
-      <c r="B33" s="6"/>
-      <c r="D33" s="2"/>
-    </row>
-    <row r="34" spans="2:4">
-      <c r="B34" s="6"/>
-      <c r="D34" s="2"/>
-    </row>
-    <row r="35" spans="2:4">
-      <c r="B35" s="6"/>
-      <c r="D35" s="2"/>
-    </row>
-    <row r="36" spans="2:4">
-      <c r="B36" s="6"/>
-      <c r="D36" s="2"/>
-    </row>
-    <row r="37" spans="2:4">
+    <row r="33" spans="1:4">
+      <c r="A33" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="6">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="6">
+        <v>3.125E-2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="6">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="6">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="B37" s="6"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="2:4">
+    <row r="38" spans="1:4">
       <c r="B38" s="6"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="2:4">
+    <row r="39" spans="1:4">
       <c r="B39" s="6"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="2:4">
+    <row r="40" spans="1:4">
       <c r="B40" s="6"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="2:4">
+    <row r="41" spans="1:4">
       <c r="B41" s="6"/>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="2:4">
+    <row r="42" spans="1:4">
       <c r="B42" s="6"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="2:4">
+    <row r="43" spans="1:4">
       <c r="B43" s="6"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="2:4">
+    <row r="44" spans="1:4">
       <c r="B44" s="6"/>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="2:4">
+    <row r="45" spans="1:4">
       <c r="B45" s="6"/>
       <c r="D45" s="2"/>
     </row>
-    <row r="46" spans="2:4">
+    <row r="46" spans="1:4">
       <c r="B46" s="6"/>
       <c r="D46" s="2"/>
     </row>
-    <row r="47" spans="2:4">
+    <row r="47" spans="1:4">
       <c r="B47" s="6"/>
       <c r="D47" s="2"/>
     </row>
-    <row r="48" spans="2:4">
+    <row r="48" spans="1:4">
       <c r="B48" s="6"/>
       <c r="D48" s="2"/>
     </row>
@@ -5057,7 +5112,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E4555F9B-702D-FD4F-A0B2-5CBE96A3F479}">
           <x14:formula1>
             <xm:f>Tätigkeiten!$B$2:$B$12</xm:f>

</xml_diff>

<commit_message>
Time to se sheet
</commit_message>
<xml_diff>
--- a/docs/Timesheets/Timesheet-Maximilian-Suitner.xlsx
+++ b/docs/Timesheets/Timesheet-Maximilian-Suitner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Projects\prodiga\docs\Timesheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6655EBC8-F056-42D3-970F-DA6EE5445C5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291BE7AD-1B50-467D-B47B-C72F1BBFC59F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="38640" windowHeight="21390" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="92">
   <si>
     <t>Datum</t>
   </si>
@@ -316,6 +316,9 @@
   </si>
   <si>
     <t>9.5.2020</t>
+  </si>
+  <si>
+    <t>30.5.2020</t>
   </si>
 </sst>
 </file>
@@ -769,7 +772,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D50" sqref="D50"/>
+      <selection pane="bottomRight" activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1482,7 +1485,7 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="8" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="B51" s="6">
         <v>8.3333333333333329E-2</v>

</xml_diff>